<commit_message>
- CompareMSExcelFiles.sct: Fix the issue where when the 'Extract workbook data to multiple files' option is enabled, all sheets of .xlsx files containing more than 10 sheets are not compared. - Specify radix to parseInt() function
</commit_message>
<xml_diff>
--- a/Testing/Data/Office/excel.xlsx
+++ b/Testing/Data/Office/excel.xlsx
@@ -1,28 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{05FD6F33-64CE-4736-AD77-41E00D3A08A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84C153C6-7E20-46A7-880B-6DB4559C36E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet7" sheetId="7" r:id="rId7"/>
+    <sheet name="Sheet8" sheetId="8" r:id="rId8"/>
+    <sheet name="Sheet9" sheetId="9" r:id="rId9"/>
+    <sheet name="Sheet10" sheetId="10" r:id="rId10"/>
+    <sheet name="Sheet11" sheetId="11" r:id="rId11"/>
+    <sheet name="Sheet12" sheetId="12" r:id="rId12"/>
+    <sheet name="Sheet13" sheetId="13" r:id="rId13"/>
+    <sheet name="Sheet14" sheetId="14" r:id="rId14"/>
+    <sheet name="Sheet15" sheetId="15" r:id="rId15"/>
+    <sheet name="Sheet16" sheetId="16" r:id="rId16"/>
+    <sheet name="Sheet17" sheetId="17" r:id="rId17"/>
+    <sheet name="Sheet18" sheetId="18" r:id="rId18"/>
+    <sheet name="Sheet19" sheetId="19" r:id="rId19"/>
+    <sheet name="Sheet20" sheetId="20" r:id="rId20"/>
   </sheets>
   <calcPr calcId="80000"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -85,7 +92,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -254,7 +261,7 @@
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
           <a:off x="685800" y="2228850"/>
-          <a:ext cx="1384300" cy="1028700"/>
+          <a:ext cx="1381125" cy="1028700"/>
           <a:chOff x="603250" y="2146300"/>
           <a:chExt cx="1231900" cy="952500"/>
         </a:xfrm>
@@ -476,8 +483,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
-          <a:off x="2743200" y="2260600"/>
-          <a:ext cx="685800" cy="996950"/>
+          <a:off x="2743200" y="2257425"/>
+          <a:ext cx="685800" cy="1000125"/>
           <a:chOff x="2438400" y="2165350"/>
           <a:chExt cx="403280" cy="920803"/>
         </a:xfrm>
@@ -969,7 +976,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:D6"/>
   <sheetViews>
@@ -1039,8 +1046,138 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A49188A-B7B0-42BB-B7FD-05451C9A0F15}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData/>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD28219A-22CA-422C-937D-F13D6D2AD4E1}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData/>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30D16640-53CB-4260-BEE3-A2DE7CB6AB3E}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData/>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C52C5F0-43C5-41D0-B454-39617CFEBA35}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData/>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2421241-B46A-4D07-9E00-8F7297B270D2}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData/>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F404D904-DA50-4BF3-B6DD-DB960A1F2C87}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData/>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E8D635F-6E1C-4EE3-940F-BF946C086D39}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData/>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93EC5C53-9909-453E-B171-12963C6EE787}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData/>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEF814B7-0FD8-46E5-8E42-59C794C0692E}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData/>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27010736-68CF-4E40-8957-287848A6BF7A}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData/>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1"/>
   <sheetViews>
@@ -1055,8 +1192,21 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A1413DB-D3B9-4A60-88BC-C915B114D278}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData/>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1"/>
   <sheetViews>
@@ -1069,4 +1219,82 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D9E140E-E0FC-4106-83B4-D45C6ED16728}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData/>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE0AECDF-EC89-4C6D-AC18-567908086EFC}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData/>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8766A06-A9C4-4458-BFFE-EE7111C825BC}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData/>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4797DC5-C038-4F40-8579-6424455B9E2B}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData/>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86830DEE-0014-49E4-9A07-4C6EF478ABE5}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData/>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A29B7AC0-45A7-4D94-B317-A4AE82B6F5E5}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData/>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>